<commit_message>
more stuff from old version: texts, data structure, card art, etc.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C861C331-EDC4-406A-AA00-027E692FDE2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2EE418-D000-499E-8A6F-936A1BECD168}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8040" yWindow="2910" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>Key</t>
   </si>
@@ -50,6 +50,444 @@
   </si>
   <si>
     <t>FLASH CARD TIME\nHUMAN BODY SYSTEM</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>newGame</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>confirmNewGameDesc</t>
+  </si>
+  <si>
+    <t>There is already a game in progress. Are you sure you want to start a new game?</t>
+  </si>
+  <si>
+    <t>organSystemExcretory</t>
+  </si>
+  <si>
+    <t>EXCRETORY SYSTEM</t>
+  </si>
+  <si>
+    <t>organSystemMuscular</t>
+  </si>
+  <si>
+    <t>MUSCULAR SYSTEM</t>
+  </si>
+  <si>
+    <t>organSystemNervous</t>
+  </si>
+  <si>
+    <t>NERVOUS SYSTEM</t>
+  </si>
+  <si>
+    <t>organSystemRespiratory</t>
+  </si>
+  <si>
+    <t>RESPIRATORY SYSTEM</t>
+  </si>
+  <si>
+    <t>organSystemReproductive</t>
+  </si>
+  <si>
+    <t>REPRODUCTIVE SYSTEM</t>
+  </si>
+  <si>
+    <t>organSystemCirculatory</t>
+  </si>
+  <si>
+    <t>CIRCULATORY SYSTEM</t>
+  </si>
+  <si>
+    <t>organSystemDigestive</t>
+  </si>
+  <si>
+    <t>DIGESTIVE SYSTEM</t>
+  </si>
+  <si>
+    <t>organKidneys</t>
+  </si>
+  <si>
+    <t>KIDNEYS</t>
+  </si>
+  <si>
+    <t>organMuscles</t>
+  </si>
+  <si>
+    <t>MUSCLES</t>
+  </si>
+  <si>
+    <t>organBrain</t>
+  </si>
+  <si>
+    <t>BRAIN</t>
+  </si>
+  <si>
+    <t>organLungs</t>
+  </si>
+  <si>
+    <t>LUNGS</t>
+  </si>
+  <si>
+    <t>organOvaries</t>
+  </si>
+  <si>
+    <t>OVARIES</t>
+  </si>
+  <si>
+    <t>organHeart</t>
+  </si>
+  <si>
+    <t>HEART</t>
+  </si>
+  <si>
+    <t>organIntestines</t>
+  </si>
+  <si>
+    <t>INTESTINES</t>
+  </si>
+  <si>
+    <t>start_intro0_0</t>
+  </si>
+  <si>
+    <t>Greetings and salutations!</t>
+  </si>
+  <si>
+    <t>start_intro0_1</t>
+  </si>
+  <si>
+    <t>I’m here to help you go over your body’s various &lt;color=#ff807b&gt;systems&lt;/color&gt;, and their associated &lt;color=#ff807b&gt;subsystems&lt;/color&gt; (&lt;color=#ffe08f&gt;organs&lt;/color&gt; and &lt;color=#ffe08f&gt;tissues&lt;/color&gt;).</t>
+  </si>
+  <si>
+    <t>start_intro0_2</t>
+  </si>
+  <si>
+    <t>As you may know, your body contains trillions of &lt;color=#ffe08f&gt;cells&lt;/color&gt;!</t>
+  </si>
+  <si>
+    <t>start_intro0_3</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ffe08f&gt;cells&lt;/color&gt; form the many &lt;color=#ffe08f&gt;tissues&lt;/color&gt; of your body.\n\nThe &lt;color=#ffe08f&gt;organs&lt;/color&gt; are made up of &lt;color=#ffe08f&gt;tissues&lt;/color&gt;, and &lt;color=#9cd395&gt;work together&lt;/color&gt; to perform the functions of your body.</t>
+  </si>
+  <si>
+    <t>start_intro1_0</t>
+  </si>
+  <si>
+    <t>Here’s an example.</t>
+  </si>
+  <si>
+    <t>start_intro2_0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ff807b&gt;circulatory system&lt;/color&gt; (also called cardiovascular system) &lt;color=#9cd395&gt;helps circulate&lt;/color&gt; &lt;color=#ffe08f&gt;blood and nutrients&lt;/color&gt; around your body. Think of it as the super highway in your body.</t>
+  </si>
+  <si>
+    <t>start_intro3_0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ffe08f&gt;heart&lt;/color&gt; is part of the &lt;color=#ff807b&gt;circulatory subsystem&lt;/color&gt;.  It &lt;color=#9cd395&gt;pumps&lt;/color&gt; &lt;color=#ffe08f&gt;oxygenated blood&lt;/color&gt; to the body and &lt;color=#ffe08f&gt;deoxygenated blood&lt;/color&gt; to the &lt;color=#ffe08f&gt;lungs&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_intro4_0</t>
+  </si>
+  <si>
+    <t>Now let’s play a little card game to match these &lt;color=#ff807b&gt;systems&lt;/color&gt; and &lt;color=#ffe08f&gt;organs&lt;/color&gt; based on their &lt;color=#9cd395&gt;functions&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_intro4_1</t>
+  </si>
+  <si>
+    <t>Simply drag the correct card into the slot to answer the question.</t>
+  </si>
+  <si>
+    <t>start_multi_questions</t>
+  </si>
+  <si>
+    <t>Now for the following questions, I need you to answer with two cards.</t>
+  </si>
+  <si>
+    <t>start_lesson_0_system_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ff807b&gt;system&lt;/color&gt; is responsible for &lt;color=#9cd395&gt;distributing&lt;/color&gt; nutrients, &lt;color=#9cd395&gt;filtering&lt;/color&gt; out wastes, and &lt;color=#9cd395&gt;transport&lt;/color&gt; immunity around the body?</t>
+  </si>
+  <si>
+    <t>start_lesson_0_system_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ff807b&gt;circulatory system&lt;/color&gt; consists of: &lt;color=#ffe08f&gt;the heart, blood vessels, blood cells&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_lesson_0_subsystem_question</t>
+  </si>
+  <si>
+    <t>Which of these is part of the &lt;color=#ff807b&gt;circulatory system&lt;/color&gt; that &lt;color=#9cd395&gt;pumps&lt;/color&gt; &lt;color=#ffe08f&gt;blood cells&lt;/color&gt; through the &lt;color=#ffe08f&gt;blood vessels&lt;/color&gt;?</t>
+  </si>
+  <si>
+    <t>start_lesson_0_subsystem_result0</t>
+  </si>
+  <si>
+    <t>Your &lt;color=#ffe08f&gt;heart&lt;/color&gt; &lt;color=#9cd395&gt;pumps&lt;/color&gt; &lt;color=#ffe08f&gt;blood cells&lt;/color&gt; through your &lt;color=#ffe08f&gt;blood vessels&lt;/color&gt;. &lt;color=#ffe08f&gt;Blood&lt;/color&gt; &lt;color=#9cd395&gt;provides&lt;/color&gt; &lt;color=#ffe08f&gt;oxygen and nutrients&lt;/color&gt;, as well as &lt;color=#9cd395&gt;assists in the removal&lt;/color&gt; of &lt;color=#ffe08f&gt;metabolic wastes&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_lesson_1_system_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ff807b&gt;system&lt;/color&gt; is responsible for the &lt;color=#9cd395&gt;digestion&lt;/color&gt; and &lt;color=#9cd395&gt;absorption&lt;/color&gt; of food?</t>
+  </si>
+  <si>
+    <t>start_lesson_1_system_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ff807b&gt;digestive system&lt;/color&gt; consists of organs working together to &lt;color=#9cd395&gt;convert&lt;/color&gt; &lt;color=#ffe08f&gt;food&lt;/color&gt; into &lt;color=#ffe08f&gt;energy and basic nutrients&lt;/color&gt; to feed the entire body.</t>
+  </si>
+  <si>
+    <t>start_lesson_1_subsystem_question</t>
+  </si>
+  <si>
+    <t>Which of these is part of the &lt;color=#ff807b&gt;digestive system&lt;/color&gt;?</t>
+  </si>
+  <si>
+    <t>start_lesson_1_subsystem_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ffe08f&gt;intestines&lt;/color&gt; consist of two major subdivisions: the small intestine and the large intestine. &lt;color=#ffe08f&gt;Chemicals&lt;/color&gt; from other organs travel here to &lt;color=#9cd395&gt;digest&lt;/color&gt; food, and &lt;color=#9cd395&gt;extract&lt;/color&gt; nutrients.</t>
+  </si>
+  <si>
+    <t>start_lesson_2_system_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ff807b&gt;system&lt;/color&gt; is responsible for the &lt;color=#9cd395&gt;storage&lt;/color&gt; and &lt;color=#9cd395&gt;discharge&lt;/color&gt; of &lt;color=#ffe08f&gt;wastes&lt;/color&gt; from the body?</t>
+  </si>
+  <si>
+    <t>start_lesson_2_system_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ff807b&gt;excretory system&lt;/color&gt; &lt;color=#9cd395&gt;removes&lt;/color&gt; &lt;color=#ffe08f&gt;wastes&lt;/color&gt;, so as to &lt;color=#9cd395&gt;prevent damage&lt;/color&gt; to the body.</t>
+  </si>
+  <si>
+    <t>start_lesson_2_subsystem_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ffe08f&gt;organ&lt;/color&gt; is responsible for the &lt;color=#9cd395&gt;production, storage, and elimination&lt;/color&gt; of &lt;color=#ffe08f&gt;urine&lt;/color&gt;?</t>
+  </si>
+  <si>
+    <t>start_lesson_2_subsystem_result0</t>
+  </si>
+  <si>
+    <t>&lt;color=#ffe08f&gt;Blood&lt;/color&gt; enters the &lt;color=#ffe08f&gt;kidneys&lt;/color&gt; in order to be &lt;color=#9cd395&gt;cleansed&lt;/color&gt; of urea and other wastes. These toxic elements eventually travel to the &lt;color=#ffe08f&gt;bladder&lt;/color&gt;, ready to be &lt;color=#9cd395&gt;extracted&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_lesson_3_system_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ff807b&gt;system&lt;/color&gt; is responsible for the &lt;color=#ffe08f&gt;voluntary&lt;/color&gt; and &lt;color=#ffe08f&gt;involuntary&lt;/color&gt; &lt;color=#9cd395&gt;movements&lt;/color&gt; in the body?</t>
+  </si>
+  <si>
+    <t>start_lesson_3_system_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ff807b&gt;muscular system&lt;/color&gt; consists of skeletal, smooth and cardiac muscles. It permits &lt;color=#9cd395&gt;movement&lt;/color&gt; of the body, &lt;color=#9cd395&gt;maintains posture&lt;/color&gt;, and &lt;color=#9cd395&gt;circulates blood&lt;/color&gt; throughout the body.</t>
+  </si>
+  <si>
+    <t>start_lesson_3_subsystem_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ffe08f&gt;organ&lt;/color&gt; is responsible for the &lt;color=#ffe08f&gt;voluntary&lt;/color&gt; and &lt;color=#ffe08f&gt;involuntary&lt;/color&gt; &lt;color=#9cd395&gt;movements&lt;/color&gt; in the body?</t>
+  </si>
+  <si>
+    <t>start_lesson_3_subsystem_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ffe08f&gt;muscles&lt;/color&gt; allow &lt;color=#9cd395&gt;movement&lt;/color&gt; of the body, &lt;color=#9cd395&gt;maintain posture&lt;/color&gt;, and &lt;color=#9cd395&gt;circulate blood&lt;/color&gt; throughout the body.</t>
+  </si>
+  <si>
+    <t>start_lesson_4_system_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ff807b&gt;system&lt;/color&gt; is responsible for &lt;color=#9cd395&gt;controlling&lt;/color&gt; and &lt;color=#9cd395&gt;coordinating&lt;/color&gt; the &lt;color=#ff807b&gt;other systems&lt;/color&gt; of the body?</t>
+  </si>
+  <si>
+    <t>start_lesson_4_system_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ff807b&gt;nervous system&lt;/color&gt; &lt;color=#9cd395&gt;coordinates&lt;/color&gt; the body's actions and &lt;color=#9cd395&gt;transmits signals&lt;/color&gt; to and from different parts of the body. These signals are transmitted via &lt;color=#ffe08f&gt;neurons&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_lesson_4_subsystem_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ffe08f&gt;organ&lt;/color&gt; is responsible for &lt;color=#9cd395&gt;controlling&lt;/color&gt; and &lt;color=#9cd395&gt;coordinating&lt;/color&gt; the &lt;color=#ff807b&gt;other systems&lt;/color&gt; of the body?</t>
+  </si>
+  <si>
+    <t>start_lesson_4_subsystem_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ffe08f&gt;brain&lt;/color&gt; is an organ that serves as the center of the &lt;color=#ff807b&gt;nervous system&lt;/color&gt;.  This is where all your &lt;color=#9cd395&gt;senses&lt;/color&gt; are processed.  There lies all of your thoughts, experiences, and feelings.</t>
+  </si>
+  <si>
+    <t>start_lesson_5_system_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ff807b&gt;system&lt;/color&gt; is involved in the &lt;color=#9cd395&gt;intake&lt;/color&gt; and &lt;color=#9cd395&gt;exchange&lt;/color&gt; of &lt;color=#ffe08f&gt;oxygen&lt;/color&gt; and &lt;color=#ffe08f&gt;carbon dioxide&lt;/color&gt; between the body and the environment?</t>
+  </si>
+  <si>
+    <t>start_lesson_5_system_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ff807b&gt;respiratory system&lt;/color&gt; works closely together with the &lt;color=#ff807b&gt;circulatory system&lt;/color&gt; with the exchange of &lt;color=#ffe08f&gt;oxygen&lt;/color&gt; and &lt;color=#ffe08f&gt;carbon dioxide&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_lesson_5_subsystem_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ffe08f&gt;organ&lt;/color&gt; is involved in the &lt;color=#9cd395&gt;intake&lt;/color&gt; and &lt;color=#9cd395&gt;exchange&lt;/color&gt; of &lt;color=#ffe08f&gt;oxygen&lt;/color&gt; and &lt;color=#ffe08f&gt;carbon dioxide&lt;/color&gt; between the body and the environment?</t>
+  </si>
+  <si>
+    <t>start_lesson_5_subsystem_result0</t>
+  </si>
+  <si>
+    <t>The passage of air into the &lt;color=#ffe08f&gt;lungs&lt;/color&gt; to &lt;color=#9cd395&gt;supply&lt;/color&gt; the body with &lt;color=#ffe08f&gt;oxygen&lt;/color&gt; is known as &lt;color=#9cd395&gt;inhalation&lt;/color&gt;, and the passage of air out of the lungs to &lt;color=#9cd395&gt;expel&lt;/color&gt; &lt;color=#ffe08f&gt;carbon dioxide&lt;/color&gt; is known as &lt;color=#9cd395&gt;exhalation&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_lesson_6_system_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ff807b&gt;system&lt;/color&gt; is responsible for the &lt;color=#9cd395&gt;continual existence&lt;/color&gt; of mankind?</t>
+  </si>
+  <si>
+    <t>start_lesson_6_system_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ff807b&gt;reproductive system&lt;/color&gt; is a system of &lt;color=#ffe08f&gt;sex organs&lt;/color&gt; in the body which work together for the purpose of &lt;color=#9cd395&gt;sexual reproduction&lt;/color&gt;. It takes two to tango.</t>
+  </si>
+  <si>
+    <t>start_lesson_6_subsystem_question</t>
+  </si>
+  <si>
+    <t>Which &lt;color=#ffe08f&gt;organ&lt;/color&gt; provides the means for reproduction?</t>
+  </si>
+  <si>
+    <t>start_lesson_6_subsystem_result0</t>
+  </si>
+  <si>
+    <t>The &lt;color=#ffe08f&gt;ovary&lt;/color&gt; ('egg' in English) is an ovum-producing reproductive organ, often found in pairs in the female body of the &lt;color=#ff807b&gt;reproductive system&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_lesson_0_system_interaction_question</t>
+  </si>
+  <si>
+    <t>Which of the &lt;color=#ff807b&gt;two systems&lt;/color&gt; work closely together in the exchange of &lt;color=#ffe08f&gt;oxygen&lt;/color&gt; and &lt;color=#ffe08f&gt;carbon dioxide&lt;/color&gt;?</t>
+  </si>
+  <si>
+    <t>start_lesson_1_system_interaction_question</t>
+  </si>
+  <si>
+    <t>Which of the &lt;color=#ff807b&gt;two systems&lt;/color&gt; work together in &lt;color=#9cd395&gt;breaking down&lt;/color&gt; the &lt;color=#ffe08f&gt;food&lt;/color&gt; we eat into &lt;color=#ffe08f&gt;nutrients&lt;/color&gt;, and then &lt;color=#9cd395&gt;deliver&lt;/color&gt; the &lt;color=#ffe08f&gt;nutrients&lt;/color&gt; to the other &lt;color=#ff807b&gt;body systems&lt;/color&gt;?</t>
+  </si>
+  <si>
+    <t>start_lesson_2_system_interaction_question</t>
+  </si>
+  <si>
+    <t>&lt;color=#ff807b&gt;One system&lt;/color&gt; &lt;color=#9cd395&gt;collects&lt;/color&gt; &lt;color=#ffe08f&gt;waste products&lt;/color&gt;, and &lt;color=#9cd395&gt;turns&lt;/color&gt; them into &lt;color=#ffe08f&gt;urine&lt;/color&gt;.\n\n&lt;color=#ff807b&gt;Another system&lt;/color&gt; lets the body &lt;color=#9cd395&gt;know&lt;/color&gt; when to release those &lt;color=#ffe08f&gt;wastes&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_lesson_3_system_interaction_question</t>
+  </si>
+  <si>
+    <t>&lt;color=#ff807b&gt;One system&lt;/color&gt; &lt;color=#9cd395&gt;brings&lt;/color&gt; in &lt;color=#ffe08f&gt;oxygen&lt;/color&gt; and &lt;color=#9cd395&gt;removes&lt;/color&gt; &lt;color=#ffe08f&gt;carbon dioxide&lt;/color&gt; that is &lt;color=#9cd395&gt;produced&lt;/color&gt; by the &lt;color=#ff807b&gt;other system&lt;/color&gt; as it &lt;color=#9cd395&gt;contracts&lt;/color&gt; and &lt;color=#9cd395&gt;relaxes&lt;/color&gt; when a person performs &lt;color=#ffe08f&gt;physical activities&lt;/color&gt;.</t>
+  </si>
+  <si>
+    <t>start_end0</t>
+  </si>
+  <si>
+    <t>Excellent! You got 'em all!</t>
+  </si>
+  <si>
+    <t>start_end1</t>
+  </si>
+  <si>
+    <t>Three cheers for victory!</t>
+  </si>
+  <si>
+    <t>start_end_score</t>
+  </si>
+  <si>
+    <t>YOU SCORED {0} OUT OF {1}</t>
+  </si>
+  <si>
+    <t>end_thanks</t>
+  </si>
+  <si>
+    <t>Thank you for playing!</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
   </si>
 </sst>
 </file>
@@ -382,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,6 +878,590 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>